<commit_message>
deploy: event logic & round reset
</commit_message>
<xml_diff>
--- a/event_deck_15.xlsx
+++ b/event_deck_15.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eba31d120ab29d09/デスクトップ/game-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="221" documentId="8_{BF624F17-91C2-4BD1-AABC-2742A4FFA852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98487385-E978-4527-9B77-9C00F3866FBA}"/>
+  <xr:revisionPtr revIDLastSave="242" documentId="8_{BF624F17-91C2-4BD1-AABC-2742A4FFA852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3500D83-0BE1-42D0-871A-0DB3DAAA8780}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="イベント15" sheetId="1" r:id="rId1"/>
@@ -194,7 +194,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>イベント</t>
+    <t>イベン+A1:D22ト名</t>
     <rPh sb="0" eb="3">
       <t>キタイチ</t>
     </rPh>
@@ -586,7 +586,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection sqref="A1:M21"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -789,7 +789,7 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -996,7 +996,7 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -1029,10 +1029,10 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M12">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -1355,11 +1355,11 @@
       </c>
       <c r="H22">
         <f>SUMPRODUCT($C$2:$C$21,H2:H21)</f>
-        <v>0.10000000000000002</v>
+        <v>2.0000000000000007E-2</v>
       </c>
       <c r="I22">
         <f>SUMPRODUCT($C$2:$C$21,I2:I21)</f>
-        <v>0.12</v>
+        <v>4.0000000000000036E-2</v>
       </c>
       <c r="J22">
         <f>SUMPRODUCT($C$2:$C$21,J2:J21)</f>
@@ -1375,11 +1375,11 @@
       </c>
       <c r="M22">
         <f>SUMPRODUCT($C$2:$C$21,M2:M21)</f>
-        <v>0.18</v>
+        <v>0.1</v>
       </c>
       <c r="N22">
         <f>AVEDEV(D22:M22)</f>
-        <v>5.1000000000000004E-2</v>
+        <v>6.8999999999999992E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>